<commit_message>
Calculations are reviewed by iteration, performance is analyzed.
</commit_message>
<xml_diff>
--- a/Project 3/Traction Motor Design.xlsx
+++ b/Project 3/Traction Motor Design.xlsx
@@ -70,9 +70,6 @@
     <t>Current Rating (A)</t>
   </si>
   <si>
-    <t>Integral, Double Layer, Distributed Winding</t>
-  </si>
-  <si>
     <t>Specific Electric Loading-q (A/m)</t>
   </si>
   <si>
@@ -112,9 +109,6 @@
     <t>Axial Length (m)</t>
   </si>
   <si>
-    <t>Airgap Clearance (m)</t>
-  </si>
-  <si>
     <t>A (mm^2)</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>rpm</t>
   </si>
   <si>
-    <t>(17AWG-1,04mm^2)</t>
-  </si>
-  <si>
     <t>Output Power Rating (W)</t>
   </si>
   <si>
@@ -194,6 +185,15 @@
   </si>
   <si>
     <t>Number of RotorSlots</t>
+  </si>
+  <si>
+    <t>Integral, Single Layer, Distributed Winding</t>
+  </si>
+  <si>
+    <t>Airgap Clearance (mm)</t>
+  </si>
+  <si>
+    <t>Slot Pitch (mm)</t>
   </si>
 </sst>
 </file>
@@ -261,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,6 +285,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1713,7 +1716,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,10 +1733,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="12"/>
       <c r="C1" s="1">
         <v>6</v>
       </c>
@@ -1741,41 +1744,41 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
       <c r="M1" s="1">
         <v>54</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="1"/>
       <c r="P1" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q1" s="1">
         <f>(Q3/Q4)^(1/3)</f>
-        <v>0.29859296910436695</v>
+        <v>0.32639302946076354</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="12"/>
       <c r="C2" s="10" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
       <c r="M2" s="1">
         <f>M1/C1</f>
         <v>9</v>
@@ -1783,18 +1786,18 @@
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
       <c r="P2" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="1">
         <f>Q1*Q4</f>
-        <v>0.22548549913135782</v>
+        <v>0.24647899574364052</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="1">
         <f>SIN(M3*N4/2)/(M3*SIN(N4/2))</f>
         <v>0.95979508052393891</v>
@@ -1815,11 +1818,11 @@
         <f>SIN(9*M3*N4/2)/(M3*SIN(9*N4/2))</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
       <c r="M3" s="1">
         <f>M2/3</f>
         <v>3</v>
@@ -1827,18 +1830,18 @@
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
       <c r="P3" s="9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="1">
         <f>(M10*2)/(PI()*M12)</f>
-        <v>2.0103782285292037E-2</v>
+        <v>2.6258001352218181E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="1">
         <f>M3*M5*C1/2</f>
         <v>18</v>
@@ -1847,11 +1850,11 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" s="1">
         <f>180/M2</f>
         <v>20</v>
@@ -1862,7 +1865,7 @@
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="Q4" s="1">
         <f>(PI()/(2*C1/2))*(C1/2)^(1/3)</f>
@@ -1870,10 +1873,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="1">
         <f>547.43*3</f>
         <v>1642.29</v>
@@ -1889,29 +1892,29 @@
         <v>13</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="1">
         <v>2</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="1">
         <f>Q6*PI()*Q1/C9</f>
-        <v>102.81403103506123</v>
+        <v>112.38638056771248</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="11"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="1">
         <v>0.7</v>
       </c>
@@ -1919,11 +1922,11 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="J6" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="J6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="1">
         <f>(M3*M5*C1/2)</f>
         <v>18</v>
@@ -1931,48 +1934,48 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q6" s="1">
         <v>60000</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="J7" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="J7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
       <c r="M7" s="1">
         <f>M8*PI()*Q1*Q2*(1/(C1/2))</f>
-        <v>5.6404895646658973E-2</v>
+        <v>5.8972216203734031E-2</v>
       </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="1">
         <f>Q5/M1</f>
-        <v>1.9039635376863191</v>
+        <v>2.0812292697724533</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="11"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="1">
         <v>1350</v>
       </c>
@@ -1980,24 +1983,29 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="J8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
+      <c r="J8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
       <c r="M8" s="1">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
+      <c r="P8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q8" s="1">
+        <f>PI()*Q1/M1</f>
+        <v>1.8988776732163922E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="1">
         <f>C10/(1.732*C8)</f>
         <v>547.42964673680615</v>
@@ -2006,11 +2014,11 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="J9" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
+      <c r="J9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
       <c r="M9" s="1">
         <f>0.18+0.0006*((C1/2)^0.4)</f>
         <v>0.1809311073443492</v>
@@ -2021,10 +2029,10 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="11"/>
+      <c r="A10" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="12"/>
       <c r="C10" s="1">
         <v>1280000</v>
       </c>
@@ -2032,11 +2040,11 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="J10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="J10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
       <c r="M10" s="2">
         <f>C10/M11</f>
         <v>8041.5129141168163</v>
@@ -2047,22 +2055,23 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="11"/>
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="12"/>
       <c r="C11" s="1">
-        <v>50</v>
+        <f>78</f>
+        <v>78</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="J11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
+      <c r="J11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
       <c r="M11" s="1">
         <f>2*PI()*N11/60</f>
         <v>159.17402778188287</v>
@@ -2071,32 +2080,32 @@
         <v>1520</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" s="11"/>
+      <c r="A12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="12"/>
       <c r="C12" s="1">
         <f>C10/'Motor Parameter Estimation'!I2</f>
-        <v>1598208.4726528006</v>
+        <v>1280742.1465866771</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="J12" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="J12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
       <c r="M12" s="1">
         <f>1/(2*4*PI()*10^-7)*M8^2</f>
-        <v>254647.90894703259</v>
+        <v>194964.80528757177</v>
       </c>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -2104,11 +2113,11 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J13" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
+      <c r="J13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
       <c r="M13" s="1">
         <v>62</v>
       </c>
@@ -2123,6 +2132,21 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
     <mergeCell ref="J13:L13"/>
     <mergeCell ref="J12:L12"/>
     <mergeCell ref="J6:L6"/>
@@ -2133,21 +2157,6 @@
     <mergeCell ref="J10:L10"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2159,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,55 +2190,57 @@
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>0.2</v>
+        <f>'Winding Design'!Q2</f>
+        <v>0.24647899574364052</v>
       </c>
       <c r="B2" s="1">
-        <v>0.115</v>
+        <f>'Winding Design'!Q1</f>
+        <v>0.32639302946076354</v>
       </c>
       <c r="C2" s="1">
         <f>'Winding Design'!Q1*2</f>
-        <v>0.59718593820873389</v>
+        <v>0.65278605892152708</v>
       </c>
       <c r="D2" s="1">
         <v>5000</v>
@@ -2245,11 +2256,12 @@
         <v>1.5</v>
       </c>
       <c r="H2" s="1">
+        <f>'Winding Design'!Q6</f>
         <v>60000</v>
       </c>
       <c r="I2" s="1">
         <f>('Winding Design'!C10-(H5+D5+50))/'Winding Design'!C10</f>
-        <v>0.80089676778861052</v>
+        <v>0.99942053395474251</v>
       </c>
       <c r="J2" s="1">
         <v>0.8</v>
@@ -2260,76 +2272,74 @@
       </c>
       <c r="L2" s="1">
         <f>(('Winding Design'!C10*I2)/(K2*M2))/1000</f>
-        <v>23254.771934277986</v>
+        <v>2923.1279250139951</v>
       </c>
       <c r="M2" s="1">
-        <f>B2^2*A2</f>
-        <v>2.6450000000000002E-3</v>
+        <f>'Winding Design'!Q3</f>
+        <v>2.6258001352218181E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>41</v>
-      </c>
       <c r="H4" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>PI()*B2/'Winding Design'!C1</f>
-        <v>6.021385919380437E-2</v>
+        <v>0.1708989905894753</v>
       </c>
       <c r="B5" s="1">
         <f>2*A2+2.3*A5+0.24</f>
-        <v>0.77849187614574999</v>
+        <v>1.1260256698430742</v>
       </c>
       <c r="C5" s="1">
-        <f>0.021*B5*'Winding Design'!M6/1.04</f>
-        <v>0.28295185498374376</v>
+        <f>0.021*B5*'Winding Design'!M6/D2</f>
+        <v>8.5127540640136406E-5</v>
       </c>
       <c r="D5" s="1">
         <f>3*'Winding Design'!C9^2*C5</f>
-        <v>254384.37200681528</v>
+        <v>76.532864460174267</v>
       </c>
       <c r="E5" s="1">
         <f>(('Winding Design'!M6^2)/('Winding Design'!M9/((2.5/1000)*A2*4*PI()*10^-7)))/10^-3</f>
-        <v>1.1251531422132568E-3</v>
+        <v>1.3866330827526255E-3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1">
         <f>PI()*(C2/2)^2*A2*7850</f>
-        <v>439.75286711930454</v>
+        <v>647.56176154672391</v>
       </c>
       <c r="H5" s="1">
         <f>G5*0.95</f>
-        <v>417.76522376333929</v>
+        <v>615.18367346938771</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:D6">

</xml_diff>

<commit_message>
Iterations and simulations are concluded. Report is finalized.
</commit_message>
<xml_diff>
--- a/Project 3/Traction Motor Design.xlsx
+++ b/Project 3/Traction Motor Design.xlsx
@@ -7,8 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Winding Design" sheetId="1" r:id="rId1"/>
-    <sheet name="Motor Parameter Estimation" sheetId="2" r:id="rId2"/>
+    <sheet name="Motor Geometry and Elect. Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Number of Poles</t>
   </si>
@@ -34,9 +33,6 @@
     <t>Number of Turns</t>
   </si>
   <si>
-    <t>Wire Size</t>
-  </si>
-  <si>
     <t>Fill Factor</t>
   </si>
   <si>
@@ -58,12 +54,6 @@
     <t>Conductors per Slot</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt; </t>
-  </si>
-  <si>
-    <t>(mm^2)</t>
-  </si>
-  <si>
     <t>Voltage Rating (V)</t>
   </si>
   <si>
@@ -73,21 +63,6 @@
     <t>Specific Electric Loading-q (A/m)</t>
   </si>
   <si>
-    <t>Full-Load Efficiency</t>
-  </si>
-  <si>
-    <t>Full-Load Power Factor</t>
-  </si>
-  <si>
-    <t>Output Coefficient</t>
-  </si>
-  <si>
-    <t>ns (rps)</t>
-  </si>
-  <si>
-    <t>D^2.L(m^3)</t>
-  </si>
-  <si>
     <t>L (m)</t>
   </si>
   <si>
@@ -106,54 +81,15 @@
     <t>Bavg (T)</t>
   </si>
   <si>
-    <t>Axial Length (m)</t>
-  </si>
-  <si>
-    <t>A (mm^2)</t>
-  </si>
-  <si>
-    <t>Specific Magnetic Loading (T)</t>
-  </si>
-  <si>
-    <t>Flux Density in Teeth (T)</t>
-  </si>
-  <si>
-    <t>Flux Density in Core (T)</t>
-  </si>
-  <si>
     <t>Torque (N.m)</t>
   </si>
   <si>
     <t>Speed (rad/s)</t>
   </si>
   <si>
-    <t>Pole Pitch (m)</t>
-  </si>
-  <si>
-    <t>l_mt (m)</t>
-  </si>
-  <si>
-    <t>Phase Resistance (ohm)</t>
-  </si>
-  <si>
     <t>wye</t>
   </si>
   <si>
-    <t>Core Mass (kg)</t>
-  </si>
-  <si>
-    <t>Core Loss (W)</t>
-  </si>
-  <si>
-    <t>Do (m)</t>
-  </si>
-  <si>
-    <t>Phase Inductance (mH)</t>
-  </si>
-  <si>
-    <t>Leakage Inductance (mH)</t>
-  </si>
-  <si>
     <t>rpm</t>
   </si>
   <si>
@@ -163,12 +99,6 @@
     <t>Input Power Rating (W)</t>
   </si>
   <si>
-    <t>Stator Copper Losses (W)</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Di^2*L</t>
   </si>
   <si>
@@ -194,6 +124,9 @@
   </si>
   <si>
     <t>Slot Pitch (mm)</t>
+  </si>
+  <si>
+    <t>Do(m)</t>
   </si>
 </sst>
 </file>
@@ -261,23 +194,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -285,6 +209,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,7 +352,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Winding Design'!$D$21:$D$40</c:f>
+              <c:f>'Motor Geometry and Elect. Data'!$D$21:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -434,7 +361,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Winding Design'!$E$21:$E$40</c:f>
+              <c:f>'Motor Geometry and Elect. Data'!$E$21:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -480,7 +407,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Winding Design'!$D$21:$D$40</c:f>
+              <c:f>'Motor Geometry and Elect. Data'!$D$21:$D$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -489,7 +416,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Winding Design'!$F$21:$F$40</c:f>
+              <c:f>'Motor Geometry and Elect. Data'!$F$21:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1716,7 +1643,7 @@
   <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,10 +1660,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="1">
         <v>6</v>
       </c>
@@ -1744,18 +1671,18 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="J1" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
+      <c r="J1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="1">
         <v>54</v>
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="1"/>
-      <c r="P1" s="8" t="s">
-        <v>23</v>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="Q1" s="1">
         <f>(Q3/Q4)^(1/3)</f>
@@ -1763,30 +1690,30 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="J2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="J2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="1">
         <f>M1/C1</f>
         <v>9</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="8" t="s">
-        <v>22</v>
+      <c r="P2" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="Q2" s="1">
         <f>Q1*Q4</f>
@@ -1794,10 +1721,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="1">
         <f>SIN(M3*N4/2)/(M3*SIN(N4/2))</f>
         <v>0.95979508052393891</v>
@@ -1818,19 +1745,19 @@
         <f>SIN(9*M3*N4/2)/(M3*SIN(9*N4/2))</f>
         <v>-0.33333333333333331</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
+      <c r="J3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="1">
         <f>M2/3</f>
         <v>3</v>
       </c>
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="9" t="s">
-        <v>49</v>
+      <c r="P3" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="Q3" s="1">
         <f>(M10*2)/(PI()*M12)</f>
@@ -1838,23 +1765,23 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="10"/>
       <c r="C4" s="1">
         <f>M3*M5*C1/2</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="J4" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="J4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
       <c r="M4" s="1">
         <f>180/M2</f>
         <v>20</v>
@@ -1864,8 +1791,8 @@
         <v>0.3490658503988659</v>
       </c>
       <c r="O4" s="1"/>
-      <c r="P4" s="9" t="s">
-        <v>51</v>
+      <c r="P4" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="Q4" s="1">
         <f>(PI()/(2*C1/2))*(C1/2)^(1/3)</f>
@@ -1873,48 +1800,36 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
+      <c r="J5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="1">
         <v>4</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="1">
-        <f>547.43*3</f>
-        <v>1642.29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1">
-        <f>('Motor Parameter Estimation'!D2*C6/M5)</f>
-        <v>1750</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="J5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="1">
-        <v>2</v>
       </c>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="9" t="s">
-        <v>52</v>
+      <c r="P5" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="Q5" s="1">
-        <f>Q6*PI()*Q1/C9</f>
-        <v>112.38638056771248</v>
+        <f>M5*M1</f>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12"/>
+      <c r="A6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="1">
         <v>0.7</v>
       </c>
@@ -1922,60 +1837,64 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="J6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="J6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="1">
         <f>(M3*M5*C1/2)</f>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="9" t="s">
-        <v>16</v>
+      <c r="P6" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="Q6" s="1">
-        <v>60000</v>
+        <f>Q5/(PI()*Q1/C9)</f>
+        <v>115316.46392145919</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12"/>
+      <c r="A7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10"/>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="J7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="J7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="1">
         <f>M8*PI()*Q1*Q2*(1/(C1/2))</f>
         <v>5.8972216203734031E-2</v>
       </c>
-      <c r="N7" s="1"/>
+      <c r="N7" s="1">
+        <f>(C8/SQRT(3))/(4.44*C11*C3*M6)</f>
+        <v>6.5135019568795596E-2</v>
+      </c>
       <c r="O7" s="1"/>
-      <c r="P7" s="6" t="s">
-        <v>53</v>
+      <c r="P7" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="Q7" s="1">
         <f>Q5/M1</f>
-        <v>2.0812292697724533</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="12"/>
+      <c r="A8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="10"/>
       <c r="C8" s="1">
         <v>1350</v>
       </c>
@@ -1983,18 +1902,18 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="J8" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
+      <c r="J8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
       <c r="M8" s="1">
         <v>0.7</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="11" t="s">
-        <v>57</v>
+      <c r="P8" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="Q8" s="1">
         <f>PI()*Q1/M1</f>
@@ -2002,10 +1921,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="12"/>
+      <c r="A9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10"/>
       <c r="C9" s="1">
         <f>C10/(1.732*C8)</f>
         <v>547.42964673680615</v>
@@ -2014,25 +1933,30 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="J9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
+      <c r="J9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
       <c r="M9" s="1">
         <f>0.18+0.0006*((C1/2)^0.4)</f>
         <v>0.1809311073443492</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
+      <c r="P9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" s="1">
+        <f>Q1*1.5</f>
+        <v>0.48958954419114531</v>
+      </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="12"/>
+      <c r="A10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="1">
         <v>1280000</v>
       </c>
@@ -2040,11 +1964,11 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="J10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="J10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="2">
         <f>C10/M11</f>
         <v>8041.5129141168163</v>
@@ -2055,10 +1979,10 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="12"/>
+      <c r="A11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
       <c r="C11" s="1">
         <f>78</f>
         <v>78</v>
@@ -2067,11 +1991,11 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="J11" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
+      <c r="J11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="1">
         <f>2*PI()*N11/60</f>
         <v>159.17402778188287</v>
@@ -2080,29 +2004,26 @@
         <v>1520</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="1">
-        <f>C10/'Motor Parameter Estimation'!I2</f>
-        <v>1280742.1465866771</v>
-      </c>
+      <c r="A12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="J12" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
+      <c r="J12" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="1">
         <f>1/(2*4*PI()*10^-7)*M8^2</f>
         <v>194964.80528757177</v>
@@ -2113,11 +2034,11 @@
       <c r="Q12" s="1"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="J13" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
+      <c r="J13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="1">
         <v>62</v>
       </c>
@@ -2127,16 +2048,21 @@
       <c r="Q13" s="1"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="5"/>
-      <c r="B61" s="5"/>
+      <c r="A61" s="4"/>
+      <c r="B61" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A10:B10"/>
@@ -2147,233 +2073,14 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="25" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.5703125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="19.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <f>'Winding Design'!Q2</f>
-        <v>0.24647899574364052</v>
-      </c>
-      <c r="B2" s="1">
-        <f>'Winding Design'!Q1</f>
-        <v>0.32639302946076354</v>
-      </c>
-      <c r="C2" s="1">
-        <f>'Winding Design'!Q1*2</f>
-        <v>0.65278605892152708</v>
-      </c>
-      <c r="D2" s="1">
-        <v>5000</v>
-      </c>
-      <c r="E2" s="1">
-        <f>0.8</f>
-        <v>0.8</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G2" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="H2" s="1">
-        <f>'Winding Design'!Q6</f>
-        <v>60000</v>
-      </c>
-      <c r="I2" s="1">
-        <f>('Winding Design'!C10-(H5+D5+50))/'Winding Design'!C10</f>
-        <v>0.99942053395474251</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="K2" s="1">
-        <f>(120*50/'Winding Design'!C1)/60</f>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="L2" s="1">
-        <f>(('Winding Design'!C10*I2)/(K2*M2))/1000</f>
-        <v>2923.1279250139951</v>
-      </c>
-      <c r="M2" s="1">
-        <f>'Winding Design'!Q3</f>
-        <v>2.6258001352218181E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <f>PI()*B2/'Winding Design'!C1</f>
-        <v>0.1708989905894753</v>
-      </c>
-      <c r="B5" s="1">
-        <f>2*A2+2.3*A5+0.24</f>
-        <v>1.1260256698430742</v>
-      </c>
-      <c r="C5" s="1">
-        <f>0.021*B5*'Winding Design'!M6/D2</f>
-        <v>8.5127540640136406E-5</v>
-      </c>
-      <c r="D5" s="1">
-        <f>3*'Winding Design'!C9^2*C5</f>
-        <v>76.532864460174267</v>
-      </c>
-      <c r="E5" s="1">
-        <f>(('Winding Design'!M6^2)/('Winding Design'!M9/((2.5/1000)*A2*4*PI()*10^-7)))/10^-3</f>
-        <v>1.3866330827526255E-3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="1">
-        <f>PI()*(C2/2)^2*A2*7850</f>
-        <v>647.56176154672391</v>
-      </c>
-      <c r="H5" s="1">
-        <f>G5*0.95</f>
-        <v>615.18367346938771</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A5:D6">
-    <cfRule type="dataBar" priority="1">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{65605CF0-8A24-4652-8E8A-FE25475B23BD}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{65605CF0-8A24-4652-8E8A-FE25475B23BD}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>A5:D6</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>